<commit_message>
updated agents to include employers
</commit_message>
<xml_diff>
--- a/agents/agent_profiles_source.xlsx
+++ b/agents/agent_profiles_source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/dev/Synthetic_Modeling/Synthetic_Modeling/agents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CA6AFA-F435-314A-8F45-50F282A89A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7851272A-82D1-0C49-B5FB-7A30125A9144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="33600" windowHeight="19420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Banks" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2009" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="630">
   <si>
     <t>swift_code</t>
   </si>
@@ -1945,6 +1945,9 @@
   </si>
   <si>
     <t>BEnt</t>
+  </si>
+  <si>
+    <t>employer</t>
   </si>
 </sst>
 </file>
@@ -2057,7 +2060,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2073,9 +2076,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2350,9 +2352,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{680087BA-8ED1-D24F-B249-1ED76B0B1B9E}" name="People" displayName="People" ref="A1:Q11" totalsRowShown="0" headerRowDxfId="12">
-  <autoFilter ref="A1:Q11" xr:uid="{680087BA-8ED1-D24F-B249-1ED76B0B1B9E}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{680087BA-8ED1-D24F-B249-1ED76B0B1B9E}" name="People" displayName="People" ref="A1:R11" totalsRowShown="0" headerRowDxfId="12">
+  <autoFilter ref="A1:R11" xr:uid="{680087BA-8ED1-D24F-B249-1ED76B0B1B9E}"/>
+  <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{454C68CE-6D61-204B-8CB8-44035D7E6904}" name="entity_id"/>
     <tableColumn id="15" xr3:uid="{6BC92FD9-3E9C-C046-8E16-AAC501BA3699}" name="type"/>
     <tableColumn id="16" xr3:uid="{BE1830A8-5950-8E45-B19C-D500345A264F}" name="sends"/>
@@ -2366,6 +2368,7 @@
     <tableColumn id="8" xr3:uid="{F9ACF06F-BD4C-2F48-810F-5FEC38C0EA74}" name="bank"/>
     <tableColumn id="9" xr3:uid="{5F4379A2-88B5-BA4A-97A7-109C85E4F3B4}" name="account_number"/>
     <tableColumn id="10" xr3:uid="{32052348-F470-2645-85B2-7E6468A98911}" name="employment_status"/>
+    <tableColumn id="18" xr3:uid="{E682BF38-44C7-4446-B451-89719FFEAB26}" name="employer"/>
     <tableColumn id="11" xr3:uid="{4EECB0F8-CF71-B743-A3CC-AE0E1DC4EEBE}" name="income_level"/>
     <tableColumn id="12" xr3:uid="{3436FD50-2241-464F-A1DD-E2A6DFCCE0A9}" name="transaction_scaler"/>
     <tableColumn id="13" xr3:uid="{97F0A11E-C7E6-0E4D-94E0-B5F1FB994AA4}" name="merchant_patterns" dataDxfId="10"/>
@@ -2402,14 +2405,7 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F4F56D53-07F6-DE4C-A300-92F755A46222}" name="Merchants" displayName="Merchants" ref="A1:K172" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:K172" xr:uid="{00000000-0001-0000-0300-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="ATM"/>
-        <filter val="BankEntity"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K172" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K172">
     <sortCondition descending="1" ref="G1:G172"/>
   </sortState>
@@ -2869,10 +2865,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2882,14 +2878,14 @@
     <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.5" customWidth="1"/>
-    <col min="13" max="13" width="18.1640625" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" customWidth="1"/>
-    <col min="15" max="15" width="16.5" customWidth="1"/>
-    <col min="16" max="16" width="52" customWidth="1"/>
-    <col min="17" max="17" width="18.6640625" customWidth="1"/>
+    <col min="13" max="14" width="18.1640625" customWidth="1"/>
+    <col min="15" max="15" width="12.83203125" customWidth="1"/>
+    <col min="16" max="16" width="16.5" customWidth="1"/>
+    <col min="17" max="17" width="52" customWidth="1"/>
+    <col min="18" max="18" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>333</v>
       </c>
@@ -2930,19 +2926,22 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>538</v>
       </c>
@@ -2983,19 +2982,22 @@
         <v>56</v>
       </c>
       <c r="N2" t="s">
+        <v>363</v>
+      </c>
+      <c r="O2" t="s">
         <v>59</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>1.5</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>539</v>
       </c>
@@ -3035,20 +3037,20 @@
       <c r="M3" t="s">
         <v>57</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>60</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>1</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>540</v>
       </c>
@@ -3089,19 +3091,22 @@
         <v>56</v>
       </c>
       <c r="N4" t="s">
+        <v>358</v>
+      </c>
+      <c r="O4" t="s">
         <v>59</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>1.5</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>541</v>
       </c>
@@ -3142,19 +3147,22 @@
         <v>56</v>
       </c>
       <c r="N5" t="s">
+        <v>365</v>
+      </c>
+      <c r="O5" t="s">
         <v>60</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>1</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="Q5" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>542</v>
       </c>
@@ -3195,19 +3203,22 @@
         <v>56</v>
       </c>
       <c r="N6" t="s">
+        <v>63</v>
+      </c>
+      <c r="O6" t="s">
         <v>60</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>1</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="Q6" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>543</v>
       </c>
@@ -3247,20 +3258,20 @@
       <c r="M7" t="s">
         <v>58</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>59</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>1.5</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="Q7" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>544</v>
       </c>
@@ -3301,19 +3312,22 @@
         <v>56</v>
       </c>
       <c r="N8" t="s">
+        <v>65</v>
+      </c>
+      <c r="O8" t="s">
         <v>61</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>0.5</v>
       </c>
-      <c r="P8" s="5" t="s">
+      <c r="Q8" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>545</v>
       </c>
@@ -3353,20 +3367,20 @@
       <c r="M9" t="s">
         <v>57</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>60</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>1</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="Q9" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>546</v>
       </c>
@@ -3377,7 +3391,7 @@
         <v>119</v>
       </c>
       <c r="D10" t="s">
-        <v>566</v>
+        <v>119</v>
       </c>
       <c r="E10" t="s">
         <v>22</v>
@@ -3407,19 +3421,22 @@
         <v>56</v>
       </c>
       <c r="N10" t="s">
+        <v>66</v>
+      </c>
+      <c r="O10" t="s">
         <v>60</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>1</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="Q10" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>547</v>
       </c>
@@ -3459,16 +3476,16 @@
       <c r="M11" t="s">
         <v>57</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>61</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>0.5</v>
       </c>
-      <c r="P11" s="5" t="s">
+      <c r="Q11" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>536</v>
       </c>
     </row>
@@ -3485,8 +3502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4882,7 +4899,7 @@
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>457</v>
       </c>
@@ -4917,7 +4934,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>393</v>
       </c>
@@ -4952,7 +4969,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>455</v>
       </c>
@@ -4987,7 +5004,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>467</v>
       </c>
@@ -5022,7 +5039,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>505</v>
       </c>
@@ -5057,7 +5074,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>508</v>
       </c>
@@ -5092,7 +5109,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -5127,7 +5144,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>411</v>
       </c>
@@ -5162,7 +5179,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>464</v>
       </c>
@@ -5197,7 +5214,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>524</v>
       </c>
@@ -5232,7 +5249,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -5267,7 +5284,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>92</v>
       </c>
@@ -5302,7 +5319,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>401</v>
       </c>
@@ -5337,7 +5354,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>428</v>
       </c>
@@ -5372,7 +5389,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>430</v>
       </c>
@@ -5407,7 +5424,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>435</v>
       </c>
@@ -5442,7 +5459,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>449</v>
       </c>
@@ -5477,7 +5494,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>463</v>
       </c>
@@ -5512,7 +5529,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>525</v>
       </c>
@@ -5547,7 +5564,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>530</v>
       </c>
@@ -5582,7 +5599,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>407</v>
       </c>
@@ -5617,7 +5634,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>490</v>
       </c>
@@ -5652,7 +5669,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>529</v>
       </c>
@@ -5687,7 +5704,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>433</v>
       </c>
@@ -5722,7 +5739,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>466</v>
       </c>
@@ -5757,7 +5774,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>492</v>
       </c>
@@ -5792,7 +5809,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>495</v>
       </c>
@@ -5827,7 +5844,7 @@
         <v>166.666666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>522</v>
       </c>
@@ -5862,7 +5879,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>531</v>
       </c>
@@ -5897,7 +5914,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>501</v>
       </c>
@@ -5932,7 +5949,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>502</v>
       </c>
@@ -5967,7 +5984,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>506</v>
       </c>
@@ -6002,7 +6019,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>458</v>
       </c>
@@ -6037,7 +6054,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>507</v>
       </c>
@@ -6072,7 +6089,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>509</v>
       </c>
@@ -6107,7 +6124,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>510</v>
       </c>
@@ -6142,7 +6159,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>511</v>
       </c>
@@ -6177,7 +6194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>512</v>
       </c>
@@ -6212,7 +6229,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>515</v>
       </c>
@@ -6247,7 +6264,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>516</v>
       </c>
@@ -6282,7 +6299,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>517</v>
       </c>
@@ -6317,7 +6334,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>518</v>
       </c>
@@ -6352,7 +6369,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>519</v>
       </c>
@@ -6387,7 +6404,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>520</v>
       </c>
@@ -6422,7 +6439,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>521</v>
       </c>
@@ -6457,7 +6474,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>375</v>
       </c>
@@ -6492,7 +6509,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>409</v>
       </c>
@@ -6527,7 +6544,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>412</v>
       </c>
@@ -6562,7 +6579,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>424</v>
       </c>
@@ -6597,7 +6614,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>480</v>
       </c>
@@ -6632,7 +6649,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>503</v>
       </c>
@@ -6667,7 +6684,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>414</v>
       </c>
@@ -6702,7 +6719,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>381</v>
       </c>
@@ -6737,7 +6754,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>382</v>
       </c>
@@ -6772,7 +6789,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>383</v>
       </c>
@@ -6807,7 +6824,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>384</v>
       </c>
@@ -6842,7 +6859,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>396</v>
       </c>
@@ -6877,7 +6894,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>436</v>
       </c>
@@ -6912,7 +6929,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>437</v>
       </c>
@@ -6947,7 +6964,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>438</v>
       </c>
@@ -6982,7 +6999,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>470</v>
       </c>
@@ -7017,7 +7034,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>472</v>
       </c>
@@ -7052,7 +7069,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>473</v>
       </c>
@@ -7087,7 +7104,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>474</v>
       </c>
@@ -7122,7 +7139,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>475</v>
       </c>
@@ -7157,7 +7174,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>477</v>
       </c>
@@ -7192,7 +7209,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>478</v>
       </c>
@@ -7227,7 +7244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>479</v>
       </c>
@@ -7262,7 +7279,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>481</v>
       </c>
@@ -7297,7 +7314,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>482</v>
       </c>
@@ -7332,7 +7349,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>91</v>
       </c>
@@ -7367,7 +7384,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>93</v>
       </c>
@@ -7402,7 +7419,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>404</v>
       </c>
@@ -7437,7 +7454,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>405</v>
       </c>
@@ -7472,7 +7489,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>415</v>
       </c>
@@ -7507,7 +7524,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>417</v>
       </c>
@@ -7542,7 +7559,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>418</v>
       </c>
@@ -7577,7 +7594,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>419</v>
       </c>
@@ -7612,7 +7629,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>450</v>
       </c>
@@ -7647,7 +7664,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>451</v>
       </c>
@@ -7682,7 +7699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>452</v>
       </c>
@@ -7717,7 +7734,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>453</v>
       </c>
@@ -7752,7 +7769,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>454</v>
       </c>
@@ -7787,7 +7804,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>484</v>
       </c>
@@ -7822,7 +7839,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>486</v>
       </c>
@@ -7857,7 +7874,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>487</v>
       </c>
@@ -7892,7 +7909,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>488</v>
       </c>
@@ -7927,7 +7944,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>94</v>
       </c>
@@ -7962,7 +7979,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>95</v>
       </c>
@@ -7997,7 +8014,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>96</v>
       </c>
@@ -8032,7 +8049,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>386</v>
       </c>
@@ -8067,7 +8084,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>388</v>
       </c>
@@ -8102,7 +8119,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>389</v>
       </c>
@@ -8137,7 +8154,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>390</v>
       </c>
@@ -8172,7 +8189,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>391</v>
       </c>
@@ -8207,7 +8224,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>392</v>
       </c>
@@ -8242,7 +8259,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>448</v>
       </c>
@@ -8277,7 +8294,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>90</v>
       </c>
@@ -8312,7 +8329,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>371</v>
       </c>
@@ -8347,7 +8364,7 @@
         <v>32000</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>387</v>
       </c>
@@ -8382,7 +8399,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>410</v>
       </c>
@@ -8417,7 +8434,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>421</v>
       </c>
@@ -8452,7 +8469,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>468</v>
       </c>
@@ -8487,7 +8504,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>485</v>
       </c>
@@ -8522,7 +8539,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>489</v>
       </c>
@@ -8557,7 +8574,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>499</v>
       </c>
@@ -8592,7 +8609,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>528</v>
       </c>
@@ -8627,7 +8644,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>406</v>
       </c>
@@ -8662,7 +8679,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>413</v>
       </c>
@@ -8697,7 +8714,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>416</v>
       </c>
@@ -8732,7 +8749,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>422</v>
       </c>
@@ -8767,7 +8784,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>423</v>
       </c>
@@ -8802,7 +8819,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>429</v>
       </c>
@@ -8837,7 +8854,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>434</v>
       </c>
@@ -8872,7 +8889,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>443</v>
       </c>
@@ -8907,7 +8924,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>444</v>
       </c>
@@ -8942,7 +8959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>445</v>
       </c>
@@ -8977,7 +8994,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>446</v>
       </c>
@@ -9012,7 +9029,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>469</v>
       </c>
@@ -9047,7 +9064,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>514</v>
       </c>
@@ -9082,7 +9099,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>526</v>
       </c>
@@ -9117,7 +9134,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>527</v>
       </c>
@@ -9152,7 +9169,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>385</v>
       </c>
@@ -9187,7 +9204,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>513</v>
       </c>
@@ -9222,7 +9239,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>431</v>
       </c>
@@ -9257,7 +9274,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>439</v>
       </c>
@@ -9292,7 +9309,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>456</v>
       </c>
@@ -9327,7 +9344,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>471</v>
       </c>
@@ -9362,7 +9379,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>491</v>
       </c>
@@ -9397,7 +9414,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>403</v>
       </c>
@@ -9432,7 +9449,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>408</v>
       </c>
@@ -9467,7 +9484,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>476</v>
       </c>
@@ -9502,7 +9519,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>500</v>
       </c>
@@ -9537,7 +9554,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>372</v>
       </c>
@@ -9572,7 +9589,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>373</v>
       </c>
@@ -9607,7 +9624,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>374</v>
       </c>
@@ -9642,7 +9659,7 @@
         <v>12500</v>
       </c>
     </row>
-    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>377</v>
       </c>
@@ -9677,7 +9694,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>378</v>
       </c>
@@ -9712,7 +9729,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>379</v>
       </c>
@@ -9747,7 +9764,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>380</v>
       </c>
@@ -9782,7 +9799,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>394</v>
       </c>
@@ -9817,7 +9834,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="143" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>395</v>
       </c>
@@ -9852,7 +9869,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>397</v>
       </c>
@@ -9887,7 +9904,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>398</v>
       </c>
@@ -9922,7 +9939,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>399</v>
       </c>
@@ -9957,7 +9974,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>400</v>
       </c>
@@ -9992,7 +10009,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>402</v>
       </c>
@@ -10027,7 +10044,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>432</v>
       </c>
@@ -10062,7 +10079,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>459</v>
       </c>
@@ -10097,7 +10114,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>460</v>
       </c>
@@ -10132,7 +10149,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>461</v>
       </c>
@@ -10167,7 +10184,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>462</v>
       </c>
@@ -10202,7 +10219,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>483</v>
       </c>
@@ -10237,7 +10254,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>493</v>
       </c>
@@ -10272,7 +10289,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>494</v>
       </c>
@@ -10307,7 +10324,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>496</v>
       </c>
@@ -10342,7 +10359,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>497</v>
       </c>
@@ -10377,7 +10394,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>498</v>
       </c>
@@ -10412,7 +10429,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>376</v>
       </c>
@@ -10447,7 +10464,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>420</v>
       </c>
@@ -10482,7 +10499,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>425</v>
       </c>
@@ -10517,7 +10534,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>426</v>
       </c>
@@ -10552,7 +10569,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>427</v>
       </c>
@@ -10587,7 +10604,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>440</v>
       </c>
@@ -10622,7 +10639,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>441</v>
       </c>
@@ -10657,7 +10674,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>442</v>
       </c>
@@ -10692,7 +10709,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>523</v>
       </c>
@@ -10727,7 +10744,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>89</v>
       </c>
@@ -10762,7 +10779,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>447</v>
       </c>
@@ -10797,7 +10814,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>465</v>
       </c>
@@ -10832,7 +10849,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>504</v>
       </c>
@@ -10881,8 +10898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B215A134-84F3-1D41-9D8B-38A50BE16B3B}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="202" zoomScaleNormal="202" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="202" zoomScaleNormal="202" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10950,7 +10967,7 @@
       <c r="H2" s="9">
         <v>211</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="9"/>
@@ -10958,36 +10975,33 @@
       <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" t="s">
         <v>605</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" t="s">
         <v>628</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="C3" t="s">
+        <v>566</v>
+      </c>
+      <c r="D3" t="s">
+        <v>566</v>
+      </c>
+      <c r="E3" t="s">
         <v>599</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3">
         <v>522</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" t="s">
         <v>588</v>
       </c>
-      <c r="H3" s="10">
-        <v>211</v>
-      </c>
-      <c r="I3" s="10" t="s">
+      <c r="H3">
+        <v>211</v>
+      </c>
+      <c r="I3" t="s">
         <v>103</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -11014,7 +11028,7 @@
       <c r="H4" s="9">
         <v>211</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" t="s">
         <v>103</v>
       </c>
       <c r="J4" s="9"/>
@@ -11022,36 +11036,33 @@
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" t="s">
         <v>607</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" t="s">
         <v>628</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="C5" t="s">
+        <v>566</v>
+      </c>
+      <c r="D5" t="s">
+        <v>566</v>
+      </c>
+      <c r="E5" t="s">
         <v>601</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5">
         <v>522</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" t="s">
         <v>588</v>
       </c>
-      <c r="H5" s="10">
-        <v>513</v>
-      </c>
-      <c r="I5" s="11" t="s">
+      <c r="H5">
+        <v>513</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
@@ -11078,7 +11089,7 @@
       <c r="H6" s="9">
         <v>513</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="10" t="s">
         <v>105</v>
       </c>
       <c r="J6" s="9"/>
@@ -11086,36 +11097,33 @@
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" t="s">
         <v>609</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" t="s">
         <v>628</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="C7" t="s">
+        <v>566</v>
+      </c>
+      <c r="D7" t="s">
+        <v>566</v>
+      </c>
+      <c r="E7" t="s">
         <v>603</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7">
         <v>522</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" t="s">
         <v>588</v>
       </c>
-      <c r="H7" s="10">
-        <v>513</v>
-      </c>
-      <c r="I7" s="11" t="s">
+      <c r="H7">
+        <v>513</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
@@ -11150,36 +11158,33 @@
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" t="s">
         <v>611</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" t="s">
         <v>628</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="E9" s="10" t="s">
+      <c r="C9" t="s">
+        <v>566</v>
+      </c>
+      <c r="D9" t="s">
+        <v>566</v>
+      </c>
+      <c r="E9" t="s">
         <v>592</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9">
         <v>522</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" t="s">
         <v>588</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9">
         <v>138</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
@@ -11214,36 +11219,33 @@
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" t="s">
         <v>613</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" t="s">
         <v>628</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="C11" t="s">
+        <v>566</v>
+      </c>
+      <c r="D11" t="s">
+        <v>566</v>
+      </c>
+      <c r="E11" t="s">
         <v>594</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11">
         <v>522</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" t="s">
         <v>588</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11">
         <v>138</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
@@ -11278,92 +11280,89 @@
       <c r="L12" s="9"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="A13" t="s">
         <v>615</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" t="s">
         <v>628</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="C13" t="s">
+        <v>566</v>
+      </c>
+      <c r="D13" t="s">
+        <v>566</v>
+      </c>
+      <c r="E13" t="s">
         <v>596</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13">
         <v>522</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" t="s">
         <v>588</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13">
         <v>138</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>616</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>628</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>566</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>566</v>
-      </c>
-      <c r="E14" s="11" t="s">
+      <c r="C14" s="10" t="s">
+        <v>566</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>566</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>597</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="10">
         <v>522</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="10" t="s">
         <v>588</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="10">
         <v>138</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="A15" t="s">
         <v>617</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" t="s">
         <v>628</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>566</v>
+      <c r="C15" t="s">
+        <v>566</v>
+      </c>
+      <c r="D15" t="s">
+        <v>119</v>
       </c>
       <c r="E15" t="s">
         <v>618</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15">
         <v>522</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" t="s">
         <v>619</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15">
         <v>138</v>
       </c>
       <c r="I15" s="9" t="s">
@@ -11371,28 +11370,28 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="A16" t="s">
         <v>620</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>628</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="D16" s="10" t="s">
+      <c r="C16" t="s">
+        <v>566</v>
+      </c>
+      <c r="D16" t="s">
         <v>566</v>
       </c>
       <c r="E16" t="s">
         <v>621</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16">
         <v>522</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" t="s">
         <v>619</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16">
         <v>138</v>
       </c>
       <c r="I16" s="9" t="s">
@@ -11400,89 +11399,89 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" t="s">
         <v>622</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" t="s">
         <v>628</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>566</v>
+      <c r="C17" t="s">
+        <v>566</v>
+      </c>
+      <c r="D17" t="s">
+        <v>119</v>
       </c>
       <c r="E17" t="s">
         <v>625</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17">
         <v>522</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" t="s">
         <v>619</v>
       </c>
-      <c r="H17" s="10">
-        <v>211</v>
-      </c>
-      <c r="I17" s="10" t="s">
+      <c r="H17">
+        <v>211</v>
+      </c>
+      <c r="I17" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" t="s">
         <v>623</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>628</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="D18" s="10" t="s">
+      <c r="C18" t="s">
+        <v>566</v>
+      </c>
+      <c r="D18" t="s">
         <v>566</v>
       </c>
       <c r="E18" t="s">
         <v>626</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18">
         <v>522</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" t="s">
         <v>619</v>
       </c>
-      <c r="H18" s="10">
-        <v>211</v>
-      </c>
-      <c r="I18" s="10" t="s">
+      <c r="H18">
+        <v>211</v>
+      </c>
+      <c r="I18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="A19" t="s">
         <v>624</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" t="s">
         <v>628</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>566</v>
+      <c r="C19" t="s">
+        <v>566</v>
+      </c>
+      <c r="D19" t="s">
+        <v>119</v>
       </c>
       <c r="E19" t="s">
         <v>627</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19">
         <v>522</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" t="s">
         <v>619</v>
       </c>
-      <c r="H19" s="10">
-        <v>513</v>
-      </c>
-      <c r="I19" s="11" t="s">
+      <c r="H19">
+        <v>513</v>
+      </c>
+      <c r="I19" s="10" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>